<commit_message>
[POI4] 2.1.1: Now ready to start with apache poi 4.1.2.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectClassStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D8181CA-09A3-AA43-A64E-D187E76B15A1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72556A4-F000-2F4A-B879-E6DEE59A71A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28300" windowHeight="17440" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -365,7 +367,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -872,35 +874,35 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,14 +1310,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1510,24 +1512,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="50"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="45"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="50"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1569,30 +1571,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E25" s="51" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1690,7 +1692,10 @@
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
-      <c r="A32" s="38"/>
+      <c r="A32" s="38">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="B32" s="39" t="s">
         <v>71</v>
       </c>
@@ -1708,8 +1713,8 @@
     </row>
     <row r="33" spans="1:7" ht="15">
       <c r="A33" s="38">
-        <f>A31+1</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B33" s="39" t="s">
         <v>40</v>
@@ -1729,7 +1734,7 @@
     <row r="34" spans="1:7" ht="15">
       <c r="A34" s="38">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" s="39" t="s">
         <v>43</v>
@@ -1749,7 +1754,7 @@
     <row r="35" spans="1:7" ht="15">
       <c r="A35" s="38">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" s="39" t="s">
         <v>47</v>
@@ -1769,7 +1774,7 @@
     <row r="36" spans="1:7" ht="15">
       <c r="A36" s="38">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B36" s="39" t="s">
         <v>50</v>
@@ -1789,7 +1794,7 @@
     <row r="37" spans="1:7" ht="15">
       <c r="A37" s="38">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" s="39" t="s">
         <v>52</v>
@@ -1809,7 +1814,7 @@
     <row r="38" spans="1:7" ht="15">
       <c r="A38" s="38">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" s="39" t="s">
         <v>53</v>
@@ -1827,7 +1832,7 @@
     <row r="39" spans="1:7" ht="45" customHeight="1">
       <c r="A39" s="38">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" s="39" t="s">
         <v>55</v>
@@ -1841,13 +1846,13 @@
       <c r="E39" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="51"/>
+      <c r="F39" s="49"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="45">
       <c r="A40" s="38">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40" s="39" t="s">
         <v>57</v>
@@ -1861,13 +1866,13 @@
       <c r="E40" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="51"/>
+      <c r="F40" s="49"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
       <c r="A41" s="38">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" s="39" t="s">
         <v>66</v>
@@ -1879,7 +1884,7 @@
       <c r="E41" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="51"/>
+      <c r="F41" s="49"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7">
@@ -1887,8 +1892,8 @@
       <c r="B42" s="22"/>
       <c r="C42" s="44"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="54"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7">
@@ -1896,6 +1901,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
@@ -1903,42 +1923,27 @@
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1951,7 +1956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
just for recording: Implementing packageSuffix and overridePackage options, and do refctoring on parsing xml.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectClassStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72556A4-F000-2F4A-B879-E6DEE59A71A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8EF72C-1C5A-EF48-93F0-57A71EA3C5BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -361,6 +361,43 @@
   </si>
   <si>
     <t>デフォルト値の変形をおこなうかどうか。※なるべく変形を利用しないことを推奨したい。※プログラムAPIとして生成する際には、このフィールドを明示的に設定してください。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>packageSuffix</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>パッケージ名の後ろに付加する文字列をしていします。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">パッケージメイ </t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ウシロニ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">フカ </t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>overridePackage</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>定義書で指定されたパッケージ名を上書きします。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ウワガキシマス。 </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -420,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -754,11 +791,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="dotted">
+        <color indexed="8"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -874,36 +926,43 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1314,10 +1373,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1512,24 +1571,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="52" t="s">
+      <c r="A19" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="50"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="52"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="52"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="50"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="52"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1571,30 +1630,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="51" t="s">
+      <c r="D25" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="51" t="s">
+      <c r="E25" s="46" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="52"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1635,7 +1694,7 @@
     </row>
     <row r="29" spans="1:7" ht="15">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A41" si="0">A28+1</f>
+        <f t="shared" ref="A29:A43" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1665,10 +1724,10 @@
       <c r="D30" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="48"/>
+      <c r="F30" s="50"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="15">
@@ -1685,10 +1744,10 @@
       <c r="D31" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E31" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="48"/>
+      <c r="F31" s="50"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
@@ -1705,10 +1764,10 @@
       <c r="D32" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="47" t="s">
+      <c r="E32" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="50"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1725,10 +1784,10 @@
       <c r="D33" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="F33" s="48"/>
+      <c r="F33" s="50"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1745,10 +1804,10 @@
       <c r="D34" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="48"/>
+      <c r="F34" s="50"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1765,10 +1824,10 @@
       <c r="D35" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="48"/>
+      <c r="F35" s="50"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1785,10 +1844,10 @@
       <c r="D36" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F36" s="48"/>
+      <c r="F36" s="50"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1805,10 +1864,10 @@
       <c r="D37" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="48"/>
+      <c r="F37" s="50"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1823,10 +1882,10 @@
         <v>35</v>
       </c>
       <c r="D38" s="40"/>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="48"/>
+      <c r="F38" s="50"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="45" customHeight="1">
@@ -1843,10 +1902,10 @@
       <c r="D39" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E39" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="49"/>
+      <c r="F39" s="51"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="45">
@@ -1863,10 +1922,10 @@
       <c r="D40" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="49"/>
+      <c r="F40" s="51"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -1881,26 +1940,79 @@
         <v>68</v>
       </c>
       <c r="D41" s="40"/>
-      <c r="E41" s="47" t="s">
+      <c r="E41" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="49"/>
+      <c r="F41" s="51"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="46"/>
+    <row r="42" spans="1:7" s="57" customFormat="1" ht="15">
+      <c r="A42" s="38">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="50"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" s="57" customFormat="1" ht="15">
+      <c r="A43" s="38">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="50"/>
       <c r="G43"/>
     </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="21"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="G45"/>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E31:F31"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -1909,25 +2021,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E41:F41"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D56" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D58" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>